<commit_message>
Added 2019 SHR data and script to create 2019 SHR and STTD data table csv and moved some files into the zoop folder
</commit_message>
<xml_diff>
--- a/NEWzooptables.xlsx
+++ b/NEWzooptables.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadams\Documents\DES docs and forms\NDFA\Manuscript\ND-FASTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40713836-E024-4BF7-9EFE-395F5D5502D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF06F9-9450-4A8C-93F0-5C4FEC916EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="2730" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="9" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
+    <workbookView xWindow="33780" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{AF2E1052-99D4-4F7E-97E0-C211836FA21F}"/>
   </bookViews>
   <sheets>
     <sheet name="adon.results" sheetId="2" r:id="rId1"/>
-    <sheet name="flowpulse_mag_dur_table" sheetId="14" r:id="rId2"/>
-    <sheet name="totalzoop_lm_anova" sheetId="1" r:id="rId3"/>
-    <sheet name="totalzoop_posthoc" sheetId="4" r:id="rId4"/>
-    <sheet name="ANOVA_cyclo" sheetId="6" r:id="rId5"/>
-    <sheet name="posthoc_cyclo" sheetId="9" r:id="rId6"/>
-    <sheet name="ANOVA_cal" sheetId="7" r:id="rId7"/>
-    <sheet name="posthoc_cal" sheetId="10" r:id="rId8"/>
-    <sheet name="ANOVA_clad" sheetId="8" r:id="rId9"/>
-    <sheet name="posthoc_clad" sheetId="13" r:id="rId10"/>
+    <sheet name="Anosim" sheetId="15" r:id="rId2"/>
+    <sheet name="flowpulse_mag_dur_table" sheetId="14" r:id="rId3"/>
+    <sheet name="totalzoop_lm_anova" sheetId="1" r:id="rId4"/>
+    <sheet name="totalzoop_posthoc" sheetId="4" r:id="rId5"/>
+    <sheet name="ANOVA_cyclo" sheetId="6" r:id="rId6"/>
+    <sheet name="posthoc_cyclo" sheetId="9" r:id="rId7"/>
+    <sheet name="ANOVA_cal" sheetId="7" r:id="rId8"/>
+    <sheet name="posthoc_cal" sheetId="10" r:id="rId9"/>
+    <sheet name="ANOVA_clad" sheetId="8" r:id="rId10"/>
+    <sheet name="posthoc_clad" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="106">
   <si>
     <t xml:space="preserve">           F</t>
   </si>
@@ -345,6 +346,24 @@
   </si>
   <si>
     <t xml:space="preserve">Aug 26 – Sep 21 </t>
+  </si>
+  <si>
+    <t>anosim_r</t>
+  </si>
+  <si>
+    <t>R_value</t>
+  </si>
+  <si>
+    <t>p_value</t>
+  </si>
+  <si>
+    <t>ANOSIM for region by year, 10000 permutations Bray-Curtis</t>
+  </si>
+  <si>
+    <t>PERMANOVA of [TaxonName zoop cpue] by region, year, sampleperiod with interactions</t>
+  </si>
+  <si>
+    <t>adon.results &lt;- adonis2(genw2[c(9:70)]~genw2$Region*genw2$SamplePeriod+genw2$Year*genw2$SamplePeriod+genw2$Region*genw2$Year, strata=genw2$StationCode,method=bray,perm=999)</t>
   </si>
 </sst>
 </file>
@@ -844,86 +863,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C329AF34-7642-45DD-AC80-3E946BA42A8C}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
+      <c r="A1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>12.354916390297401</v>
-      </c>
-      <c r="D2">
-        <v>9.3421638659728801E-2</v>
-      </c>
-      <c r="E2">
-        <v>45.270796632738502</v>
-      </c>
-      <c r="F2">
-        <v>1E-3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2.3908725709781602</v>
-      </c>
-      <c r="D3">
-        <v>1.80785710199373E-2</v>
-      </c>
-      <c r="E3">
-        <v>4.3803091221461301</v>
-      </c>
-      <c r="F3">
-        <v>1E-3</v>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>10.994764995959001</v>
+        <v>12.354916390297401</v>
       </c>
       <c r="D4">
-        <v>8.3136860675784199E-2</v>
+        <v>9.3421638659728801E-2</v>
       </c>
       <c r="E4">
-        <v>40.2869395820194</v>
+        <v>45.270796632738502</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
@@ -931,19 +924,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1.8486074702172</v>
+        <v>2.3908725709781602</v>
       </c>
       <c r="D5">
-        <v>1.39782361653157E-2</v>
+        <v>1.80785710199373E-2</v>
       </c>
       <c r="E5">
-        <v>3.3868271623305302</v>
+        <v>4.3803091221461301</v>
       </c>
       <c r="F5">
         <v>1E-3</v>
@@ -951,39 +944,39 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1.0243274345248901</v>
+        <v>10.994764995959001</v>
       </c>
       <c r="D6">
-        <v>7.7454467868825197E-3</v>
+        <v>8.3136860675784199E-2</v>
       </c>
       <c r="E6">
-        <v>1.8766666446293401</v>
+        <v>40.2869395820194</v>
       </c>
       <c r="F6">
-        <v>8.9999999999999993E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>3.2040963868979002</v>
+        <v>1.8486074702172</v>
       </c>
       <c r="D7">
-        <v>2.4227758847707798E-2</v>
+        <v>1.39782361653157E-2</v>
       </c>
       <c r="E7">
-        <v>11.7404271579579</v>
+        <v>3.3868271623305302</v>
       </c>
       <c r="F7">
         <v>1E-3</v>
@@ -991,41 +984,81 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>368</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>100.431394404521</v>
+        <v>1.0243274345248901</v>
       </c>
       <c r="D8">
-        <v>0.75941148784464296</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
+        <v>7.7454467868825197E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.8766666446293401</v>
+      </c>
+      <c r="F8">
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3.2040963868979002</v>
+      </c>
+      <c r="D9">
+        <v>2.4227758847707798E-2</v>
+      </c>
+      <c r="E9">
+        <v>11.7404271579579</v>
+      </c>
+      <c r="F9">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>368</v>
+      </c>
+      <c r="C10">
+        <v>100.431394404521</v>
+      </c>
+      <c r="D10">
+        <v>0.75941148784464296</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>377</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>132.24897965339599</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1035,10 +1068,195 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581420B1-334D-4801-9E0F-AB9FD07C8D35}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>71.600700000000003</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>61.19</v>
+      </c>
+      <c r="E6" s="6">
+        <v>6.9260000000000002E-12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>8.2349999999999994</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>30.54</v>
+      </c>
+      <c r="E7">
+        <v>7.3921000000000004E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>17.22</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>333.48</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.6820000000000003E-15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>1.7024999999999999</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>333.1</v>
+      </c>
+      <c r="E9">
+        <v>0.18380650000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>4.9337</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>333.51</v>
+      </c>
+      <c r="E10">
+        <v>2.264E-4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>4.6285999999999996</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>333.38</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3.4939999999999999E-6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0.49869999999999998</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>333.23</v>
+      </c>
+      <c r="E12">
+        <v>0.60778109999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D368C0-DCD5-45DB-9924-E738418A8B9A}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
@@ -1671,6 +1889,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27575DC5-E8B3-4281-93C6-BDF935A4CF95}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2014</v>
+      </c>
+      <c r="B4">
+        <v>0.28367199999999998</v>
+      </c>
+      <c r="C4">
+        <v>1.9997999999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2015</v>
+      </c>
+      <c r="B5">
+        <v>0.32816679999999998</v>
+      </c>
+      <c r="C5">
+        <v>9.9989999999999996E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2016</v>
+      </c>
+      <c r="B6">
+        <v>0.28499099999999999</v>
+      </c>
+      <c r="C6">
+        <v>9.9989999999999996E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2017</v>
+      </c>
+      <c r="B7">
+        <v>0.1723085</v>
+      </c>
+      <c r="C7">
+        <v>2.9996999999999999E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2018</v>
+      </c>
+      <c r="B8">
+        <v>0.25141419999999998</v>
+      </c>
+      <c r="C8">
+        <v>9.9989999999999996E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2019</v>
+      </c>
+      <c r="B9">
+        <v>0.54593349999999996</v>
+      </c>
+      <c r="C9">
+        <v>9.9989999999999996E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDD3603-B090-4E50-AB92-1557FECDBEFA}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -1903,7 +2226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96480CFD-F304-412C-B39C-F642C6CD3F54}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2058,7 +2381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C2019C-D9D2-4366-B353-52FA64F823A2}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -2705,7 +3028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D4700E-FBDC-4708-9E67-08379A0E9B65}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -2903,7 +3226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB4343-2B3A-4546-8374-BA8176CE4411}">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -3554,7 +3877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5DB659-8E39-4FD5-9EB8-C9D952203A8F}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -3745,7 +4068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A0460-4DAE-480E-BE49-2A986203EA97}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -4208,189 +4531,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581420B1-334D-4801-9E0F-AB9FD07C8D35}">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>71.600700000000003</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>61.19</v>
-      </c>
-      <c r="E6" s="6">
-        <v>6.9260000000000002E-12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7">
-        <v>8.2349999999999994</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>30.54</v>
-      </c>
-      <c r="E7">
-        <v>7.3921000000000004E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <v>17.22</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>333.48</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3.6820000000000003E-15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9">
-        <v>1.7024999999999999</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>333.1</v>
-      </c>
-      <c r="E9">
-        <v>0.18380650000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10">
-        <v>4.9337</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>333.51</v>
-      </c>
-      <c r="E10">
-        <v>2.264E-4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11">
-        <v>4.6285999999999996</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>333.38</v>
-      </c>
-      <c r="E11" s="6">
-        <v>3.4939999999999999E-6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12">
-        <v>0.49869999999999998</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>333.23</v>
-      </c>
-      <c r="E12">
-        <v>0.60778109999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>